<commit_message>
added tables and text
</commit_message>
<xml_diff>
--- a/wyniki.xlsx
+++ b/wyniki.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dawid\Desktop\Studia\Magisterka 2 semestr\Projektowanie systemow z dostepem w jezyku naturalnym\Jezyki_Naturalne\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC78D732-3DBB-402E-975E-DFE721EEED56}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF47FFEC-C442-44B9-BBDD-F5625A8F9F48}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{6AD73322-5D71-49CF-B30D-D77AD795EF39}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6AD73322-5D71-49CF-B30D-D77AD795EF39}"/>
   </bookViews>
   <sheets>
     <sheet name="dictation.io" sheetId="1" r:id="rId1"/>
@@ -1433,7 +1433,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -2376,7 +2375,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.94444444444444431</c:v>
+                  <c:v>0.94444444444444453</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2416,6 +2415,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-78D7-44EE-87CE-3F12CE81747E}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:val>
             <c:numRef>
@@ -2891,7 +2895,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Dic</c:v>
+            <c:v>Dictation.io</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -2925,7 +2929,7 @@
           <c:idx val="2"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Spee</c:v>
+            <c:v>Speechnotes</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -8941,8 +8945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D6A9181-5867-45AD-A24F-7D6B34911748}">
   <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="P33" sqref="P33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9217,7 +9221,7 @@
         <v>1</v>
       </c>
       <c r="K8" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L8" s="3">
         <v>1</v>
@@ -9227,7 +9231,7 @@
       </c>
       <c r="N8" s="4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="O8" s="4"/>
     </row>
@@ -9248,7 +9252,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" s="3">
         <v>1</v>
@@ -9273,7 +9277,7 @@
       </c>
       <c r="N9" s="4">
         <f t="shared" si="0"/>
-        <v>0.83333333333333337</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="O9" s="4">
         <f>AVERAGE(B7:M9)</f>
@@ -9283,7 +9287,7 @@
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="N10" s="5">
         <f>AVERAGE(N4:N9)</f>
-        <v>0.94444444444444431</v>
+        <v>0.94444444444444453</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -9747,7 +9751,7 @@
         <v>1</v>
       </c>
       <c r="N26" s="4">
-        <f t="shared" ref="N26:N30" si="2">AVERAGE(B26:M26)</f>
+        <f t="shared" ref="N26:N29" si="2">AVERAGE(B26:M26)</f>
         <v>0.91666666666666663</v>
       </c>
       <c r="O26" s="4"/>
@@ -9959,7 +9963,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E270DD4C-09B8-4742-885E-9ECB8612FC0E}">
   <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
@@ -10972,7 +10976,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B738FA5-91E3-4EA5-9FC3-86268909B9B7}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S22" sqref="S22"/>
     </sheetView>
   </sheetViews>

</xml_diff>